<commit_message>
Rework activity diagram and performance test
</commit_message>
<xml_diff>
--- a/Auswertung.xlsx
+++ b/Auswertung.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Bachelor\Thesis\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93B55DD-3440-4008-B5AA-D081A563788F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FCEB96-EBFC-42FF-A4D2-471B5E58A2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27345" yWindow="1575" windowWidth="20550" windowHeight="18285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Copy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -79,12 +80,31 @@
   <si>
     <t>Variante D Postgres No Flag</t>
   </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Anfragen pro Sekunde</t>
+  </si>
+  <si>
+    <t>Difference A to D MongoDB</t>
+  </si>
+  <si>
+    <t>Difference A to D Postgres No Flag</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,15 +113,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,18 +135,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -140,6 +192,1994 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Vergleich</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> der Anfragen pro Sekunde zwischen Varianten</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$T$23:$T$28</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>141</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$S$23:$S$28</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Variante A MongoDB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Variante D MongoDB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Variante D MongoDB No Flag</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Variante A Postgres</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Variante D Postgres</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Variante D Postgres No Flag</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$T$23:$T$28</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>273.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>214.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>245.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>170.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130.36000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DABE-49EE-AF22-C2D1F62F971B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="671528456"/>
+        <c:axId val="671527472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="671528456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="671527472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="671527472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#0\ &quot;Req/Sec&quot;" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="671528456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Vergleich</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> der Anfragen pro Sekunde zwischen Varianten</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Copy!$T$23:$T$28</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>19,95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19,63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20,63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19,25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18,75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19,57</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Copy!$S$23:$S$28</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Variante A MongoDB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Variante D MongoDB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Variante D MongoDB No Flag</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Variante A Postgres</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Variante D Postgres</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Variante D Postgres No Flag</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Copy!$T$23:$T$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>19.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F41D-4787-8FE3-D8B4C44FBD7D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="671528456"/>
+        <c:axId val="671527472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="671528456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="671527472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="671527472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#0\ &quot;Req/Sec&quot;" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="671528456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D44E3D0-9FC6-49D0-B081-88AC7FBE679D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E37BBF28-2C93-488F-8266-96E1E82CC37C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FB7D0FC-B7E9-4AE0-A882-93788592A882}" name="Tabelle1" displayName="Tabelle1" ref="B2:J56" totalsRowShown="0">
   <autoFilter ref="B2:J56" xr:uid="{6FB7D0FC-B7E9-4AE0-A882-93788592A882}"/>
@@ -151,9 +2191,29 @@
     <tableColumn id="5" xr3:uid="{B938FE91-0C8A-455C-B70D-15CBFD9A7331}" name="Max"/>
     <tableColumn id="6" xr3:uid="{7FA4F3FA-00D3-49F9-93ED-D63462C76CAC}" name="ResTime Mean"/>
     <tableColumn id="7" xr3:uid="{1D48DA23-6B7F-4EA5-A553-B10831B7C375}" name="ResTime Median"/>
-    <tableColumn id="8" xr3:uid="{C14CBF4C-580A-4893-A3B5-7908133312F1}" name="Request/Sec" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{109F78A7-EC26-4844-9533-B12C6777C360}" name="Time Taken" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{C14CBF4C-580A-4893-A3B5-7908133312F1}" name="Request/Sec" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{109F78A7-EC26-4844-9533-B12C6777C360}" name="Time Taken" dataDxfId="2">
       <calculatedColumnFormula>(D3/I3)*1000</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3540483-EA70-422C-BDEB-91C3ED851884}" name="Tabelle13" displayName="Tabelle13" ref="B2:J56" totalsRowShown="0">
+  <autoFilter ref="B2:J56" xr:uid="{6FB7D0FC-B7E9-4AE0-A882-93788592A882}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{714A75AE-9E56-4278-A0CF-A59C2EDEBBB6}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{38F87D15-35D0-46D2-B5E9-FE17459E4D87}" name="Pre-Data"/>
+    <tableColumn id="3" xr3:uid="{B5BC4A8A-5213-4BBE-AF8D-76273A8060EB}" name="Count"/>
+    <tableColumn id="4" xr3:uid="{C7B2C0A8-8FC2-457C-AC7D-CFAC080BF9C8}" name="Min"/>
+    <tableColumn id="5" xr3:uid="{D461E7D7-9C24-421C-A463-58564CD34589}" name="Max"/>
+    <tableColumn id="6" xr3:uid="{48E2B47B-03B0-4C07-9A96-E025DBF060BB}" name="ResTime Mean"/>
+    <tableColumn id="7" xr3:uid="{195EBA5B-041E-4686-BDAC-41795E72EA52}" name="ResTime Median"/>
+    <tableColumn id="8" xr3:uid="{53271210-2913-4FF6-8D11-45EC0A55F238}" name="Request/Sec" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{63071E46-7F04-49DF-BE39-E99BD8768568}" name="Time Taken" dataDxfId="0">
+      <calculatedColumnFormula>(D3/I3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -423,10 +2483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J56"/>
+  <dimension ref="B2:X56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,9 +2497,13 @@
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="28.28515625" customWidth="1"/>
+    <col min="19" max="19" width="22.42578125" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" customWidth="1"/>
+    <col min="21" max="21" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -468,7 +2532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -497,8 +2561,20 @@
         <f>(D3/I3)*1000</f>
         <v>1054.0006703444265</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>94.67</v>
+      </c>
+      <c r="O3">
+        <v>237.64</v>
+      </c>
+      <c r="P3">
+        <v>273.32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -527,8 +2603,20 @@
         <f t="shared" ref="J4:J56" si="0">(D4/I4)*1000</f>
         <v>1063.9995744001703</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>82.99</v>
+      </c>
+      <c r="O4">
+        <v>186.34</v>
+      </c>
+      <c r="P4">
+        <v>214.23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -557,8 +2645,23 @@
         <f t="shared" si="0"/>
         <v>1050.9997635250531</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="4">
+        <f>(N4-N3)/N3</f>
+        <v>-0.12337593746699067</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" ref="O5" si="1">(O4-O3)/O3</f>
+        <v>-0.21587274869550574</v>
+      </c>
+      <c r="P5" s="4">
+        <f>(P4-P3)/P3</f>
+        <v>-0.21619347285233428</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -588,7 +2691,7 @@
         <v>4343.9958158632298</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -617,8 +2720,20 @@
         <f t="shared" si="0"/>
         <v>4264.9997910150105</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>82.99</v>
+      </c>
+      <c r="O7">
+        <v>186.34</v>
+      </c>
+      <c r="P7">
+        <v>214.23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -647,8 +2762,20 @@
         <f t="shared" si="0"/>
         <v>4027.9994296352806</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8">
+        <v>87.32</v>
+      </c>
+      <c r="O8">
+        <v>212.34</v>
+      </c>
+      <c r="P8">
+        <v>245.32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -677,8 +2804,23 @@
         <f t="shared" si="0"/>
         <v>36736.005877760945</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="4">
+        <f>(N8-N7)/N7</f>
+        <v>5.2174960838655242E-2</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" ref="O9:P9" si="2">(O8-O7)/O7</f>
+        <v>0.13952989159600729</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.14512439901040938</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -708,7 +2850,7 @@
         <v>37083.996364284998</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -737,8 +2879,20 @@
         <f t="shared" si="0"/>
         <v>35958.999548714557</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>94.67</v>
+      </c>
+      <c r="O11">
+        <v>237.64</v>
+      </c>
+      <c r="P11">
+        <v>273.32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -767,8 +2921,20 @@
         <f t="shared" si="0"/>
         <v>1199.0005131722196</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12">
+        <v>87.32</v>
+      </c>
+      <c r="O12">
+        <v>212.34</v>
+      </c>
+      <c r="P12">
+        <v>245.32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -797,8 +2963,23 @@
         <f t="shared" si="0"/>
         <v>1218.0000925680069</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="4">
+        <f>(N12-N11)/N11</f>
+        <v>-7.7638111334108043E-2</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" ref="O13" si="3">(O12-O11)/O11</f>
+        <v>-0.10646355832351449</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" ref="P13" si="4">(P12-P11)/P11</f>
+        <v>-0.10244402165959315</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -828,7 +3009,7 @@
         <v>1198.0000587020029</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -857,8 +3038,20 @@
         <f t="shared" si="0"/>
         <v>5495.0006484100768</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15">
+        <v>94.67</v>
+      </c>
+      <c r="O15">
+        <v>237.64</v>
+      </c>
+      <c r="P15">
+        <v>273.32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -887,8 +3080,20 @@
         <f t="shared" si="0"/>
         <v>5358.9993676380745</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16">
+        <v>74</v>
+      </c>
+      <c r="O16">
+        <v>149.26</v>
+      </c>
+      <c r="P16">
+        <v>170.18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -917,8 +3122,23 @@
         <f t="shared" si="0"/>
         <v>5250.9976895610171</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N17" s="4">
+        <f>(N16-N15)/N15</f>
+        <v>-0.21833738248653217</v>
+      </c>
+      <c r="O17" s="4">
+        <f t="shared" ref="O17" si="5">(O16-O15)/O15</f>
+        <v>-0.37190708634909947</v>
+      </c>
+      <c r="P17" s="4">
+        <f>(P16-P15)/P15</f>
+        <v>-0.37735987121322989</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -948,7 +3168,7 @@
         <v>48261.989243367832</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -977,8 +3197,20 @@
         <f t="shared" si="0"/>
         <v>45591.007629655134</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19">
+        <v>74</v>
+      </c>
+      <c r="O19">
+        <v>149.26</v>
+      </c>
+      <c r="P19">
+        <v>170.18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -1007,8 +3239,20 @@
         <f t="shared" si="0"/>
         <v>46262.006725570536</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20">
+        <v>68.37</v>
+      </c>
+      <c r="O20">
+        <v>126.56</v>
+      </c>
+      <c r="P20">
+        <v>130.36000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -1037,8 +3281,23 @@
         <f t="shared" si="0"/>
         <v>1163.0003081950817</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" s="4">
+        <f>(N20-N19)/N19</f>
+        <v>-7.6081081081081026E-2</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" ref="O21" si="6">(O20-O19)/O19</f>
+        <v>-0.15208361248827543</v>
+      </c>
+      <c r="P21" s="4">
+        <f>(P20-P19)/P19</f>
+        <v>-0.23398754260195082</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -1067,8 +3326,11 @@
         <f t="shared" si="0"/>
         <v>1141.0002464560534</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="T22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -1097,8 +3359,26 @@
         <f t="shared" si="0"/>
         <v>1131.9900384876614</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N23">
+        <v>74</v>
+      </c>
+      <c r="O23">
+        <v>149.26</v>
+      </c>
+      <c r="P23">
+        <v>170.18</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T23" s="6">
+        <v>273.32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>11</v>
       </c>
@@ -1127,8 +3407,26 @@
         <f t="shared" si="0"/>
         <v>4683.0006607713931</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24">
+        <v>65.81</v>
+      </c>
+      <c r="O24">
+        <v>132.85</v>
+      </c>
+      <c r="P24">
+        <v>140.56</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T24" s="6">
+        <v>214.23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>11</v>
       </c>
@@ -1157,8 +3455,29 @@
         <f t="shared" si="0"/>
         <v>4758.0009354229833</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="4">
+        <f>(N24-N23)/N23</f>
+        <v>-0.11067567567567564</v>
+      </c>
+      <c r="O25" s="4">
+        <f t="shared" ref="O25" si="7">(O24-O23)/O23</f>
+        <v>-0.10994238241993835</v>
+      </c>
+      <c r="P25" s="4">
+        <f>(P24-P23)/P23</f>
+        <v>-0.17405100481842756</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T25" s="6">
+        <v>245.32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -1187,8 +3506,14 @@
         <f t="shared" si="0"/>
         <v>4687.9995649536404</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="S26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T26" s="6">
+        <v>170.18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>11</v>
       </c>
@@ -1217,8 +3542,26 @@
         <f t="shared" si="0"/>
         <v>40301.000109618719</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N27">
+        <v>68.37</v>
+      </c>
+      <c r="O27">
+        <v>126.56</v>
+      </c>
+      <c r="P27">
+        <v>130.36000000000001</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T27" s="6">
+        <v>130.36000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>11</v>
       </c>
@@ -1247,8 +3590,26 @@
         <f t="shared" si="0"/>
         <v>41172.002215053719</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28">
+        <v>65.81</v>
+      </c>
+      <c r="O28">
+        <v>132.85</v>
+      </c>
+      <c r="P28">
+        <v>140.56</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T28" s="6">
+        <v>140.56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>11</v>
       </c>
@@ -1277,8 +3638,23 @@
         <f t="shared" si="0"/>
         <v>40827.991671089701</v>
       </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="4">
+        <f>(N28-N27)/N27</f>
+        <v>-3.7443323094924708E-2</v>
+      </c>
+      <c r="O29" s="4">
+        <f t="shared" ref="O29" si="8">(O28-O27)/O27</f>
+        <v>4.9699747155499303E-2</v>
+      </c>
+      <c r="P29" s="4">
+        <f>(P28-P27)/P27</f>
+        <v>7.8244860386621568E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>12</v>
       </c>
@@ -1308,7 +3684,7 @@
         <v>1348.9997167100594</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -1338,7 +3714,7 @@
         <v>1359.000319365075</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>12</v>
       </c>
@@ -1367,8 +3743,41 @@
         <f t="shared" si="0"/>
         <v>1346.0000915280061</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="5">
+        <v>0</v>
+      </c>
+      <c r="O32" s="5">
+        <v>0</v>
+      </c>
+      <c r="P32" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>94.67</v>
+      </c>
+      <c r="R32">
+        <v>237.64</v>
+      </c>
+      <c r="S32">
+        <v>273.32</v>
+      </c>
+      <c r="U32" t="s">
+        <v>17</v>
+      </c>
+      <c r="V32" s="4">
+        <v>-7.7638111334108043E-2</v>
+      </c>
+      <c r="W32" s="4">
+        <v>-0.10646355832351449</v>
+      </c>
+      <c r="X32" s="4">
+        <v>-0.10244402165959315</v>
+      </c>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>12</v>
       </c>
@@ -1397,8 +3806,44 @@
         <f t="shared" si="0"/>
         <v>6895.0015375853427</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N33" s="4">
+        <f>(Q33-Q32)/Q32</f>
+        <v>-0.12337593746699067</v>
+      </c>
+      <c r="O33" s="4">
+        <f>(R33-R32)/R32</f>
+        <v>-0.21587274869550574</v>
+      </c>
+      <c r="P33" s="4">
+        <f>(S33-S32)/S32</f>
+        <v>-0.21619347285233428</v>
+      </c>
+      <c r="Q33">
+        <v>82.99</v>
+      </c>
+      <c r="R33">
+        <v>186.34</v>
+      </c>
+      <c r="S33">
+        <v>214.23</v>
+      </c>
+      <c r="U33" t="s">
+        <v>18</v>
+      </c>
+      <c r="V33" s="4">
+        <v>-0.11067567567567564</v>
+      </c>
+      <c r="W33" s="4">
+        <v>-0.10994238241993835</v>
+      </c>
+      <c r="X33" s="4">
+        <v>-0.17405100481842756</v>
+      </c>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>12</v>
       </c>
@@ -1427,8 +3872,32 @@
         <f t="shared" si="0"/>
         <v>6694.0005020500375</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N34" s="4">
+        <f>(Q34-Q32)/Q32</f>
+        <v>-7.7638111334108043E-2</v>
+      </c>
+      <c r="O34" s="4">
+        <f>(R34-R32)/R32</f>
+        <v>-0.10646355832351449</v>
+      </c>
+      <c r="P34" s="4">
+        <f t="shared" ref="P34" si="9">(S34-S32)/S32</f>
+        <v>-0.10244402165959315</v>
+      </c>
+      <c r="Q34">
+        <v>87.32</v>
+      </c>
+      <c r="R34">
+        <v>212.34</v>
+      </c>
+      <c r="S34">
+        <v>245.32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>12</v>
       </c>
@@ -1457,8 +3926,32 @@
         <f t="shared" si="0"/>
         <v>6520.0014083203041</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" s="4">
+        <f>(Q35-Q32)/Q32</f>
+        <v>-0.21833738248653217</v>
+      </c>
+      <c r="O35" s="4">
+        <f t="shared" ref="O35:P35" si="10">(R35-R32)/R32</f>
+        <v>-0.37190708634909947</v>
+      </c>
+      <c r="P35" s="4">
+        <f t="shared" si="10"/>
+        <v>-0.37735987121322989</v>
+      </c>
+      <c r="Q35">
+        <v>74</v>
+      </c>
+      <c r="R35">
+        <v>149.26</v>
+      </c>
+      <c r="S35">
+        <v>170.18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>12</v>
       </c>
@@ -1487,8 +3980,32 @@
         <f t="shared" si="0"/>
         <v>58005.986217777681</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N36" s="4">
+        <f>(Q36-Q32)/Q32</f>
+        <v>-0.27780711946762432</v>
+      </c>
+      <c r="O36" s="4">
+        <f>(R36-R32)/R32</f>
+        <v>-0.46742972563541485</v>
+      </c>
+      <c r="P36" s="4">
+        <f>(S36-S32)/S32</f>
+        <v>-0.52304990487340841</v>
+      </c>
+      <c r="Q36">
+        <v>68.37</v>
+      </c>
+      <c r="R36">
+        <v>126.56</v>
+      </c>
+      <c r="S36">
+        <v>130.36000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>12</v>
       </c>
@@ -1517,8 +4034,32 @@
         <f t="shared" si="0"/>
         <v>59893.007132059283</v>
       </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N37" s="4">
+        <f>(Q37-Q32)/Q32</f>
+        <v>-0.30484842083025243</v>
+      </c>
+      <c r="O37" s="4">
+        <f t="shared" ref="O37:P37" si="11">(R37-R32)/R32</f>
+        <v>-0.44096111765696011</v>
+      </c>
+      <c r="P37" s="4">
+        <f t="shared" si="11"/>
+        <v>-0.48573101126884238</v>
+      </c>
+      <c r="Q37">
+        <v>65.81</v>
+      </c>
+      <c r="R37">
+        <v>132.85</v>
+      </c>
+      <c r="S37">
+        <v>140.56</v>
+      </c>
+    </row>
+    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>12</v>
       </c>
@@ -1547,8 +4088,11 @@
         <f t="shared" si="0"/>
         <v>58422.988277427401</v>
       </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>13</v>
       </c>
@@ -1578,7 +4122,7 @@
         <v>1444.999002950688</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>13</v>
       </c>
@@ -1608,7 +4152,7 @@
         <v>1465.0018385773076</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>13</v>
       </c>
@@ -1638,7 +4182,7 @@
         <v>1477.9999704400004</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>13</v>
       </c>
@@ -1668,7 +4212,7 @@
         <v>7773.9944338199866</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>13</v>
       </c>
@@ -1698,7 +4242,7 @@
         <v>7871.4621713270963</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>13</v>
       </c>
@@ -1728,7 +4272,7 @@
         <v>8065.1665456891678</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>13</v>
       </c>
@@ -1758,7 +4302,7 @@
         <v>75684.986974613756</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>13</v>
       </c>
@@ -1788,7 +4332,7 @@
         <v>76075.016051828396</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>13</v>
       </c>
@@ -1818,7 +4362,7 @@
         <v>78430.019246726719</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>14</v>
       </c>
@@ -2090,8 +4634,1507 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9051846-7276-40B2-9DDD-5F7652959633}">
+  <dimension ref="B2:X56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="28.28515625" customWidth="1"/>
+    <col min="19" max="19" width="22.42578125" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" customWidth="1"/>
+    <col min="21" max="21" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>3000</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="e">
+        <f t="shared" ref="J3:J34" si="0">(D3/I3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3">
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>3000</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <v>19.63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="4" t="e">
+        <f>(N4-N3)/N3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O5" s="4" t="e">
+        <f t="shared" ref="O5" si="1">(O4-O3)/O3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="4">
+        <f>(P4-P3)/P3</f>
+        <v>-1.604010025062658E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>1000</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>19.63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8">
+        <v>20.63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <v>10000</v>
+      </c>
+      <c r="E9">
+        <v>487</v>
+      </c>
+      <c r="F9">
+        <v>543</v>
+      </c>
+      <c r="G9">
+        <v>501.47800000000001</v>
+      </c>
+      <c r="H9">
+        <v>499</v>
+      </c>
+      <c r="I9" s="1">
+        <v>19.9008</v>
+      </c>
+      <c r="J9" s="1">
+        <f>(D9/I9)</f>
+        <v>502.49236211609582</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="4" t="e">
+        <f>(N8-N7)/N7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="4" t="e">
+        <f t="shared" ref="O9:P9" si="2">(O8-O7)/O7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="2"/>
+        <v>5.0942435048395317E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10">
+        <v>10000</v>
+      </c>
+      <c r="E10">
+        <v>487</v>
+      </c>
+      <c r="F10">
+        <v>544</v>
+      </c>
+      <c r="G10">
+        <v>499.24</v>
+      </c>
+      <c r="H10">
+        <v>497</v>
+      </c>
+      <c r="I10" s="1">
+        <v>19.995000000000001</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>500.12503125781444</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+      <c r="D11">
+        <v>10000</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="e">
+        <f>(D11/I11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11">
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12">
+        <v>20.63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>1000</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="4" t="e">
+        <f>(N12-N11)/N11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" s="4" t="e">
+        <f t="shared" ref="O13:P13" si="3">(O12-O11)/O11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="3"/>
+        <v>3.4085213032581441E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>1000</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>1000</v>
+      </c>
+      <c r="D15">
+        <v>1000</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15">
+        <v>19.63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>1000</v>
+      </c>
+      <c r="D16">
+        <v>1000</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16">
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>1000</v>
+      </c>
+      <c r="D17">
+        <v>1000</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N17" s="4" t="e">
+        <f>(N16-N15)/N15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" s="4" t="e">
+        <f t="shared" ref="O17" si="4">(O16-O15)/O15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="4">
+        <f>(P16-P15)/P15</f>
+        <v>-1.9358125318390169E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>1000</v>
+      </c>
+      <c r="D18">
+        <v>10000</v>
+      </c>
+      <c r="E18">
+        <v>496</v>
+      </c>
+      <c r="F18">
+        <v>594</v>
+      </c>
+      <c r="G18">
+        <v>508.22</v>
+      </c>
+      <c r="H18">
+        <v>506</v>
+      </c>
+      <c r="I18" s="1">
+        <v>19.639600000000002</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="0"/>
+        <v>509.1753396199515</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>1000</v>
+      </c>
+      <c r="D19">
+        <v>10000</v>
+      </c>
+      <c r="E19">
+        <v>496</v>
+      </c>
+      <c r="F19">
+        <v>582</v>
+      </c>
+      <c r="G19">
+        <v>509.01</v>
+      </c>
+      <c r="H19">
+        <v>508</v>
+      </c>
+      <c r="I19" s="1">
+        <v>19.607900000000001</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="0"/>
+        <v>509.99852100428905</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P19">
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>1000</v>
+      </c>
+      <c r="D20">
+        <v>10000</v>
+      </c>
+      <c r="E20">
+        <v>496</v>
+      </c>
+      <c r="F20">
+        <v>601</v>
+      </c>
+      <c r="G20">
+        <v>508.22</v>
+      </c>
+      <c r="H20">
+        <v>507</v>
+      </c>
+      <c r="I20" s="1">
+        <v>19.636299999999999</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="0"/>
+        <v>509.26090964183686</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P20">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>1000</v>
+      </c>
+      <c r="D21">
+        <v>100</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" s="4" t="e">
+        <f>(N20-N19)/N19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="4" t="e">
+        <f t="shared" ref="O21" si="5">(O20-O19)/O19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="4">
+        <f>(P20-P19)/P19</f>
+        <v>-2.5974025974025976E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>1000</v>
+      </c>
+      <c r="D22">
+        <v>100</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>1000</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P23">
+        <v>19.25</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T23">
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>1000</v>
+      </c>
+      <c r="D24">
+        <v>1000</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P24">
+        <v>19.57</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T24">
+        <v>19.63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>1000</v>
+      </c>
+      <c r="D25">
+        <v>1000</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="4" t="e">
+        <f>(N24-N23)/N23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O25" s="4" t="e">
+        <f t="shared" ref="O25" si="6">(O24-O23)/O23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P25" s="4">
+        <f>(P24-P23)/P23</f>
+        <v>1.6623376623376637E-2</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T25">
+        <v>20.63</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>1000</v>
+      </c>
+      <c r="D26">
+        <v>1000</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T26">
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>1000</v>
+      </c>
+      <c r="D27">
+        <v>10000</v>
+      </c>
+      <c r="E27">
+        <v>467</v>
+      </c>
+      <c r="F27">
+        <v>588</v>
+      </c>
+      <c r="G27">
+        <v>482.05</v>
+      </c>
+      <c r="H27">
+        <v>481</v>
+      </c>
+      <c r="I27" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="0"/>
+        <v>483.09178743961354</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P27">
+        <v>18.75</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T27">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>1000</v>
+      </c>
+      <c r="D28">
+        <v>10000</v>
+      </c>
+      <c r="E28">
+        <v>468</v>
+      </c>
+      <c r="F28">
+        <v>557</v>
+      </c>
+      <c r="G28">
+        <v>484.14</v>
+      </c>
+      <c r="H28">
+        <v>483</v>
+      </c>
+      <c r="I28" s="1">
+        <v>20.607900000000001</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="0"/>
+        <v>485.25080187695011</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P28">
+        <v>19.57</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T28">
+        <v>19.57</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>1000</v>
+      </c>
+      <c r="D29">
+        <v>10000</v>
+      </c>
+      <c r="E29">
+        <v>467</v>
+      </c>
+      <c r="F29">
+        <v>562</v>
+      </c>
+      <c r="G29">
+        <v>484.99</v>
+      </c>
+      <c r="H29">
+        <v>484</v>
+      </c>
+      <c r="I29" s="1">
+        <v>20.58</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="0"/>
+        <v>485.90864917395533</v>
+      </c>
+      <c r="M29" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="4" t="e">
+        <f>(N28-N27)/N27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O29" s="4" t="e">
+        <f t="shared" ref="O29" si="7">(O28-O27)/O27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P29" s="4">
+        <f>(P28-P27)/P27</f>
+        <v>4.3733333333333346E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>1000</v>
+      </c>
+      <c r="D30">
+        <v>100</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>1000</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>1000</v>
+      </c>
+      <c r="D32">
+        <v>100</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="5">
+        <v>0</v>
+      </c>
+      <c r="O32" s="5">
+        <v>0</v>
+      </c>
+      <c r="P32" s="5">
+        <v>0</v>
+      </c>
+      <c r="U32" t="s">
+        <v>17</v>
+      </c>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>1000</v>
+      </c>
+      <c r="D33">
+        <v>1000</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N33" s="4" t="e">
+        <f>(Q33-Q32)/Q32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O33" s="4" t="e">
+        <f>(R33-R32)/R32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P33" s="4" t="e">
+        <f>(S33-S32)/S32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U33" t="s">
+        <v>18</v>
+      </c>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>1000</v>
+      </c>
+      <c r="D34">
+        <v>1000</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N34" s="4" t="e">
+        <f>(Q34-Q32)/Q32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O34" s="4" t="e">
+        <f>(R34-R32)/R32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P34" s="4" t="e">
+        <f t="shared" ref="P34" si="8">(S34-S32)/S32</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>1000</v>
+      </c>
+      <c r="D35">
+        <v>1000</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1" t="e">
+        <f t="shared" ref="J35:J66" si="9">(D35/I35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" s="4" t="e">
+        <f>(Q35-Q32)/Q32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O35" s="4" t="e">
+        <f t="shared" ref="O35:P35" si="10">(R35-R32)/R32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P35" s="4" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>1000</v>
+      </c>
+      <c r="D36">
+        <v>10000</v>
+      </c>
+      <c r="E36">
+        <v>503</v>
+      </c>
+      <c r="F36">
+        <v>614</v>
+      </c>
+      <c r="G36">
+        <v>517.15</v>
+      </c>
+      <c r="H36">
+        <v>515</v>
+      </c>
+      <c r="I36" s="1">
+        <v>19.286999999999999</v>
+      </c>
+      <c r="J36" s="1">
+        <f t="shared" si="9"/>
+        <v>518.48395292165708</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N36" s="4" t="e">
+        <f>(Q36-Q32)/Q32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O36" s="4" t="e">
+        <f>(R36-R32)/R32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P36" s="4" t="e">
+        <f>(S36-S32)/S32</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>1000</v>
+      </c>
+      <c r="D37">
+        <v>10000</v>
+      </c>
+      <c r="E37">
+        <v>503</v>
+      </c>
+      <c r="F37">
+        <v>603</v>
+      </c>
+      <c r="G37">
+        <v>518.04999999999995</v>
+      </c>
+      <c r="H37">
+        <v>516</v>
+      </c>
+      <c r="I37" s="1">
+        <v>19.266300000000001</v>
+      </c>
+      <c r="J37" s="1">
+        <f t="shared" si="9"/>
+        <v>519.04101981179565</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N37" s="4" t="e">
+        <f>(Q37-Q32)/Q32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O37" s="4" t="e">
+        <f t="shared" ref="O37:P37" si="11">(R37-R32)/R32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P37" s="4" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>1000</v>
+      </c>
+      <c r="D38">
+        <v>10000</v>
+      </c>
+      <c r="E38">
+        <v>505</v>
+      </c>
+      <c r="F38">
+        <v>596</v>
+      </c>
+      <c r="G38">
+        <v>519.53</v>
+      </c>
+      <c r="H38">
+        <v>518</v>
+      </c>
+      <c r="I38" s="1">
+        <v>19.207799999999999</v>
+      </c>
+      <c r="J38" s="1">
+        <f t="shared" si="9"/>
+        <v>520.62183071460561</v>
+      </c>
+      <c r="M38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39">
+        <v>1000</v>
+      </c>
+      <c r="D39">
+        <v>100</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40">
+        <v>1000</v>
+      </c>
+      <c r="D40">
+        <v>100</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>1000</v>
+      </c>
+      <c r="D41">
+        <v>100</v>
+      </c>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42">
+        <v>1000</v>
+      </c>
+      <c r="D42">
+        <v>1000</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>1000</v>
+      </c>
+      <c r="D43">
+        <v>1000</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44">
+        <v>1000</v>
+      </c>
+      <c r="D44">
+        <v>1000</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <v>1000</v>
+      </c>
+      <c r="D45">
+        <v>10000</v>
+      </c>
+      <c r="E45">
+        <v>517</v>
+      </c>
+      <c r="F45">
+        <v>615</v>
+      </c>
+      <c r="G45">
+        <v>532.66999999999996</v>
+      </c>
+      <c r="H45">
+        <v>531</v>
+      </c>
+      <c r="I45" s="1">
+        <v>18.732299999999999</v>
+      </c>
+      <c r="J45" s="1">
+        <f t="shared" si="9"/>
+        <v>533.83727572161456</v>
+      </c>
+    </row>
+    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46">
+        <v>1000</v>
+      </c>
+      <c r="D46">
+        <v>10000</v>
+      </c>
+      <c r="E46">
+        <v>517</v>
+      </c>
+      <c r="F46">
+        <v>600</v>
+      </c>
+      <c r="G46">
+        <v>533.41999999999996</v>
+      </c>
+      <c r="H46">
+        <v>532</v>
+      </c>
+      <c r="I46" s="1">
+        <v>18.7136</v>
+      </c>
+      <c r="J46" s="1">
+        <f t="shared" si="9"/>
+        <v>534.37072503419972</v>
+      </c>
+    </row>
+    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47">
+        <v>1000</v>
+      </c>
+      <c r="D47">
+        <v>10000</v>
+      </c>
+      <c r="E47">
+        <v>516</v>
+      </c>
+      <c r="F47">
+        <v>616</v>
+      </c>
+      <c r="G47">
+        <v>531.24</v>
+      </c>
+      <c r="H47">
+        <v>529</v>
+      </c>
+      <c r="I47" s="1">
+        <v>18.798100000000002</v>
+      </c>
+      <c r="J47" s="1">
+        <f t="shared" si="9"/>
+        <v>531.96865640676447</v>
+      </c>
+      <c r="S47">
+        <v>440</v>
+      </c>
+      <c r="T47">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48">
+        <v>1000</v>
+      </c>
+      <c r="D48">
+        <v>100</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49">
+        <v>1000</v>
+      </c>
+      <c r="D49">
+        <v>100</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <v>1000</v>
+      </c>
+      <c r="D50">
+        <v>100</v>
+      </c>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51">
+        <v>1000</v>
+      </c>
+      <c r="D51">
+        <v>1000</v>
+      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <v>1000</v>
+      </c>
+      <c r="D52">
+        <v>1000</v>
+      </c>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53">
+        <v>1000</v>
+      </c>
+      <c r="D53">
+        <v>1000</v>
+      </c>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54">
+        <v>1000</v>
+      </c>
+      <c r="D54">
+        <v>10000</v>
+      </c>
+      <c r="E54">
+        <v>488</v>
+      </c>
+      <c r="F54">
+        <v>603</v>
+      </c>
+      <c r="G54">
+        <v>510.4</v>
+      </c>
+      <c r="H54">
+        <v>510</v>
+      </c>
+      <c r="I54" s="1">
+        <v>19.5413</v>
+      </c>
+      <c r="J54" s="1">
+        <f t="shared" si="9"/>
+        <v>511.7366807735412</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>1000</v>
+      </c>
+      <c r="D55">
+        <v>10000</v>
+      </c>
+      <c r="E55">
+        <v>488</v>
+      </c>
+      <c r="F55">
+        <v>584</v>
+      </c>
+      <c r="G55">
+        <v>509.24</v>
+      </c>
+      <c r="H55">
+        <v>509</v>
+      </c>
+      <c r="I55" s="1">
+        <v>19.588000000000001</v>
+      </c>
+      <c r="J55" s="1">
+        <f t="shared" si="9"/>
+        <v>510.51664284255662</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <v>1000</v>
+      </c>
+      <c r="D56">
+        <v>10000</v>
+      </c>
+      <c r="E56">
+        <v>488</v>
+      </c>
+      <c r="F56">
+        <v>574</v>
+      </c>
+      <c r="G56">
+        <v>510.18</v>
+      </c>
+      <c r="H56">
+        <v>510</v>
+      </c>
+      <c r="I56" s="1">
+        <v>19.5657</v>
+      </c>
+      <c r="J56" s="1">
+        <f t="shared" si="9"/>
+        <v>511.09850401467878</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add load test results to thesis
</commit_message>
<xml_diff>
--- a/Auswertung.xlsx
+++ b/Auswertung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Bachelor\Thesis\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FCEB96-EBFC-42FF-A4D2-471B5E58A2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8219866B-A0CB-4F98-B911-CFF7169F28AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27345" yWindow="1575" windowWidth="20550" windowHeight="18285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28425" yWindow="1050" windowWidth="20550" windowHeight="18285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -696,9 +696,6 @@
                 <c:pt idx="1">
                   <c:v>19,63</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>20,63</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>19,25</c:v>
                 </c:pt>
@@ -816,9 +813,6 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19.63</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20.63</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>19.25</c:v>
@@ -2485,8 +2479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:X56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,7 +2681,7 @@
         <v>230.2028</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="0"/>
+        <f>(D6/I6)*1000</f>
         <v>4343.9958158632298</v>
       </c>
     </row>
@@ -2717,7 +2711,7 @@
         <v>234.4666</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="0"/>
+        <f>(D7/I7)*1000</f>
         <v>4264.9997910150105</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -2759,7 +2753,7 @@
         <v>248.26220000000001</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="0"/>
+        <f>(D8/I8)*1000</f>
         <v>4027.9994296352806</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -4643,10 +4637,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9051846-7276-40B2-9DDD-5F7652959633}">
-  <dimension ref="B2:X56"/>
+  <dimension ref="B2:X65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4702,10 +4696,24 @@
       <c r="D3">
         <v>100</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="e">
+      <c r="E3">
+        <v>493</v>
+      </c>
+      <c r="F3">
+        <v>589</v>
+      </c>
+      <c r="G3">
+        <v>505.13</v>
+      </c>
+      <c r="H3">
+        <v>502</v>
+      </c>
+      <c r="I3" s="1">
+        <v>16.826499999999999</v>
+      </c>
+      <c r="J3" s="1">
         <f t="shared" ref="J3:J34" si="0">(D3/I3)</f>
-        <v>#DIV/0!</v>
+        <v>5.9430065670222572</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>9</v>
@@ -4724,10 +4732,24 @@
       <c r="D4">
         <v>100</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E4">
+        <v>492</v>
+      </c>
+      <c r="F4">
+        <v>566</v>
+      </c>
+      <c r="G4">
+        <v>504.6</v>
+      </c>
+      <c r="H4">
+        <v>502</v>
+      </c>
+      <c r="I4" s="1">
+        <v>16.826499999999999</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9430065670222572</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
@@ -4746,10 +4768,24 @@
       <c r="D5">
         <v>100</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E5">
+        <v>492</v>
+      </c>
+      <c r="F5">
+        <v>566</v>
+      </c>
+      <c r="G5">
+        <v>505.23</v>
+      </c>
+      <c r="H5">
+        <v>502.5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>16.843499999999999</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9370083414967203</v>
       </c>
       <c r="M5" t="s">
         <v>15</v>
@@ -4912,10 +4948,24 @@
       <c r="D11">
         <v>10000</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1" t="e">
+      <c r="E11">
+        <v>485</v>
+      </c>
+      <c r="F11">
+        <v>543</v>
+      </c>
+      <c r="G11">
+        <v>501.35</v>
+      </c>
+      <c r="H11">
+        <v>499</v>
+      </c>
+      <c r="I11" s="1">
+        <v>19.98</v>
+      </c>
+      <c r="J11" s="1">
         <f>(D11/I11)</f>
-        <v>#DIV/0!</v>
+        <v>500.50050050050049</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>9</v>
@@ -4934,10 +4984,24 @@
       <c r="D12">
         <v>100</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E12">
+        <v>503</v>
+      </c>
+      <c r="F12">
+        <v>581</v>
+      </c>
+      <c r="G12">
+        <v>513.42999999999995</v>
+      </c>
+      <c r="H12">
+        <v>511</v>
+      </c>
+      <c r="I12" s="1">
+        <v>16.605799999999999</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="0"/>
+        <v>6.0219923159378057</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>11</v>
@@ -4956,10 +5020,24 @@
       <c r="D13">
         <v>100</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E13">
+        <v>500</v>
+      </c>
+      <c r="F13">
+        <v>583</v>
+      </c>
+      <c r="G13">
+        <v>514.34</v>
+      </c>
+      <c r="H13">
+        <v>513.5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>16.591999999999999</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>6.0270009643201545</v>
       </c>
       <c r="M13" t="s">
         <v>15</v>
@@ -4987,10 +5065,24 @@
       <c r="D14">
         <v>100</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E14">
+        <v>499</v>
+      </c>
+      <c r="F14">
+        <v>605</v>
+      </c>
+      <c r="G14">
+        <v>512.41999999999996</v>
+      </c>
+      <c r="H14">
+        <v>509</v>
+      </c>
+      <c r="I14" s="1">
+        <v>16.6722</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9980086611245067</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
@@ -5180,10 +5272,24 @@
       <c r="D21">
         <v>100</v>
       </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E21">
+        <v>499</v>
+      </c>
+      <c r="F21">
+        <v>570</v>
+      </c>
+      <c r="G21">
+        <v>510.25</v>
+      </c>
+      <c r="H21">
+        <v>508</v>
+      </c>
+      <c r="I21" s="1">
+        <v>16.652799999999999</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="0"/>
+        <v>6.0049961568024601</v>
       </c>
       <c r="M21" t="s">
         <v>15</v>
@@ -5211,10 +5317,24 @@
       <c r="D22">
         <v>100</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E22">
+        <v>495</v>
+      </c>
+      <c r="F22">
+        <v>583</v>
+      </c>
+      <c r="G22">
+        <v>509.38</v>
+      </c>
+      <c r="H22">
+        <v>506</v>
+      </c>
+      <c r="I22" s="1">
+        <v>16.764500000000002</v>
+      </c>
+      <c r="J22" s="1">
+        <f>(D22/I22)</f>
+        <v>5.9649855349100775</v>
       </c>
       <c r="T22" t="s">
         <v>16</v>
@@ -5230,10 +5350,24 @@
       <c r="D23">
         <v>100</v>
       </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E23">
+        <v>496</v>
+      </c>
+      <c r="F23">
+        <v>584</v>
+      </c>
+      <c r="G23">
+        <v>511.24</v>
+      </c>
+      <c r="H23">
+        <v>510</v>
+      </c>
+      <c r="I23" s="1">
+        <v>16.550799999999999</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="0"/>
+        <v>6.0420040118906639</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>12</v>
@@ -5309,9 +5443,6 @@
       <c r="S25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="T25">
-        <v>20.63</v>
-      </c>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -5346,23 +5477,23 @@
         <v>10000</v>
       </c>
       <c r="E27">
-        <v>467</v>
+        <v>492</v>
       </c>
       <c r="F27">
-        <v>588</v>
+        <v>564</v>
       </c>
       <c r="G27">
-        <v>482.05</v>
+        <v>507.04</v>
       </c>
       <c r="H27">
-        <v>481</v>
+        <v>506</v>
       </c>
       <c r="I27" s="1">
-        <v>20.7</v>
+        <v>19.688099999999999</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="0"/>
-        <v>483.09178743961354</v>
+        <f>(D27/I27)</f>
+        <v>507.92102843849841</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>13</v>
@@ -5388,23 +5519,23 @@
         <v>10000</v>
       </c>
       <c r="E28">
-        <v>468</v>
+        <v>492</v>
       </c>
       <c r="F28">
-        <v>557</v>
+        <v>570</v>
       </c>
       <c r="G28">
-        <v>484.14</v>
+        <v>507.43</v>
       </c>
       <c r="H28">
-        <v>483</v>
+        <v>507</v>
       </c>
       <c r="I28" s="1">
-        <v>20.607900000000001</v>
+        <v>19.666699999999999</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="0"/>
-        <v>485.25080187695011</v>
+        <f>(D28/I28)</f>
+        <v>508.47371445133149</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>14</v>
@@ -5430,23 +5561,23 @@
         <v>10000</v>
       </c>
       <c r="E29">
-        <v>467</v>
+        <v>492</v>
       </c>
       <c r="F29">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="G29">
-        <v>484.99</v>
+        <v>506.5</v>
       </c>
       <c r="H29">
-        <v>484</v>
+        <v>505</v>
       </c>
       <c r="I29" s="1">
-        <v>20.58</v>
+        <v>19.704000000000001</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="0"/>
-        <v>485.90864917395533</v>
+        <f>(D29/I29)</f>
+        <v>507.51116524563537</v>
       </c>
       <c r="M29" t="s">
         <v>15</v>
@@ -5474,10 +5605,24 @@
       <c r="D30">
         <v>100</v>
       </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E30">
+        <v>510</v>
+      </c>
+      <c r="F30">
+        <v>593</v>
+      </c>
+      <c r="G30">
+        <v>521.29999999999995</v>
+      </c>
+      <c r="H30">
+        <v>518</v>
+      </c>
+      <c r="I30" s="1">
+        <v>16.345199999999998</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="0"/>
+        <v>6.1180040623546983</v>
       </c>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.25">
@@ -5490,10 +5635,24 @@
       <c r="D31">
         <v>100</v>
       </c>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E31">
+        <v>507</v>
+      </c>
+      <c r="F31">
+        <v>588</v>
+      </c>
+      <c r="G31">
+        <v>524.47</v>
+      </c>
+      <c r="H31">
+        <v>522</v>
+      </c>
+      <c r="I31" s="1">
+        <v>16.254899999999999</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="0"/>
+        <v>6.1519910919168996</v>
       </c>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.25">
@@ -5506,10 +5665,24 @@
       <c r="D32">
         <v>100</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E32">
+        <v>512</v>
+      </c>
+      <c r="F32">
+        <v>603</v>
+      </c>
+      <c r="G32">
+        <v>526.37</v>
+      </c>
+      <c r="H32">
+        <v>524</v>
+      </c>
+      <c r="I32" s="1">
+        <v>16.1447</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="0"/>
+        <v>6.1939831647537584</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>9</v>
@@ -5610,7 +5783,7 @@
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1" t="e">
-        <f t="shared" ref="J35:J66" si="9">(D35/I35)</f>
+        <f t="shared" ref="J35:J56" si="9">(D35/I35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M35" s="3" t="s">
@@ -5762,10 +5935,24 @@
       <c r="D39">
         <v>100</v>
       </c>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1" t="e">
+      <c r="E39">
+        <v>523</v>
+      </c>
+      <c r="F39">
+        <v>613</v>
+      </c>
+      <c r="G39">
+        <v>540.15</v>
+      </c>
+      <c r="H39">
+        <v>536</v>
+      </c>
+      <c r="I39" s="1">
+        <v>15.951499999999999</v>
+      </c>
+      <c r="J39" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>6.2690029150863555</v>
       </c>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
@@ -5778,10 +5965,24 @@
       <c r="D40">
         <v>100</v>
       </c>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1" t="e">
+      <c r="E40">
+        <v>523</v>
+      </c>
+      <c r="F40">
+        <v>598</v>
+      </c>
+      <c r="G40">
+        <v>535.04</v>
+      </c>
+      <c r="H40">
+        <v>534</v>
+      </c>
+      <c r="I40" s="1">
+        <v>16.04</v>
+      </c>
+      <c r="J40" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>6.2344139650872821</v>
       </c>
     </row>
     <row r="41" spans="2:24" x14ac:dyDescent="0.25">
@@ -5794,10 +5995,24 @@
       <c r="D41">
         <v>100</v>
       </c>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1" t="e">
+      <c r="E41">
+        <v>525</v>
+      </c>
+      <c r="F41">
+        <v>593</v>
+      </c>
+      <c r="G41">
+        <v>538.01</v>
+      </c>
+      <c r="H41">
+        <v>537</v>
+      </c>
+      <c r="I41" s="1">
+        <v>15.9541</v>
+      </c>
+      <c r="J41" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>6.2679812712719611</v>
       </c>
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.25">
@@ -5954,10 +6169,24 @@
       <c r="D48">
         <v>100</v>
       </c>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1" t="e">
+      <c r="E48">
+        <v>495</v>
+      </c>
+      <c r="F48">
+        <v>561</v>
+      </c>
+      <c r="G48">
+        <v>512.74</v>
+      </c>
+      <c r="H48">
+        <v>511</v>
+      </c>
+      <c r="I48" s="1">
+        <v>16.666499999999999</v>
+      </c>
+      <c r="J48" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>6.0000600006000067</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
@@ -5970,10 +6199,24 @@
       <c r="D49">
         <v>100</v>
       </c>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1" t="e">
+      <c r="E49">
+        <v>496</v>
+      </c>
+      <c r="F49">
+        <v>578</v>
+      </c>
+      <c r="G49">
+        <v>514.22</v>
+      </c>
+      <c r="H49">
+        <v>510</v>
+      </c>
+      <c r="I49" s="1">
+        <v>16.4528</v>
+      </c>
+      <c r="J49" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>6.0779928036565209</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -5986,10 +6229,24 @@
       <c r="D50">
         <v>100</v>
       </c>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1" t="e">
+      <c r="E50">
+        <v>497</v>
+      </c>
+      <c r="F50">
+        <v>579</v>
+      </c>
+      <c r="G50">
+        <v>513.16999999999996</v>
+      </c>
+      <c r="H50">
+        <v>511</v>
+      </c>
+      <c r="I50" s="1">
+        <v>16.498899999999999</v>
+      </c>
+      <c r="J50" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>6.0610101279479238</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
@@ -6051,23 +6308,23 @@
         <v>10000</v>
       </c>
       <c r="E54">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="F54">
         <v>603</v>
       </c>
       <c r="G54">
-        <v>510.4</v>
+        <v>518.98</v>
       </c>
       <c r="H54">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="I54" s="1">
-        <v>19.5413</v>
+        <v>19.2148</v>
       </c>
       <c r="J54" s="1">
         <f t="shared" si="9"/>
-        <v>511.7366807735412</v>
+        <v>520.43216687136999</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -6081,23 +6338,23 @@
         <v>10000</v>
       </c>
       <c r="E55">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="F55">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="G55">
-        <v>509.24</v>
+        <v>515.75</v>
       </c>
       <c r="H55">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="I55" s="1">
-        <v>19.588000000000001</v>
+        <v>19.340599999999998</v>
       </c>
       <c r="J55" s="1">
         <f t="shared" si="9"/>
-        <v>510.51664284255662</v>
+        <v>517.04704093978478</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
@@ -6111,23 +6368,89 @@
         <v>10000</v>
       </c>
       <c r="E56">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="F56">
-        <v>574</v>
+        <v>592</v>
       </c>
       <c r="G56">
-        <v>510.18</v>
+        <v>517.57000000000005</v>
       </c>
       <c r="H56">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="I56" s="1">
-        <v>19.5657</v>
+        <v>19.2729</v>
       </c>
       <c r="J56" s="1">
         <f t="shared" si="9"/>
-        <v>511.09850401467878</v>
+        <v>518.863274338579</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <v>19.96</v>
+      </c>
+      <c r="D60">
+        <v>16.829999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>19.63</v>
+      </c>
+      <c r="D61">
+        <v>16.62</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62">
+        <v>19.690000000000001</v>
+      </c>
+      <c r="D62">
+        <v>16.66</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63">
+        <v>19.25</v>
+      </c>
+      <c r="D63">
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64">
+        <v>18.75</v>
+      </c>
+      <c r="D64">
+        <v>15.98</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65">
+        <v>19.28</v>
+      </c>
+      <c r="D65">
+        <v>16.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalize Performance Test Results
</commit_message>
<xml_diff>
--- a/Auswertung.xlsx
+++ b/Auswertung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Bachelor\Thesis\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8219866B-A0CB-4F98-B911-CFF7169F28AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D4C1A6-4D2E-40FF-B00C-144B4A686F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28425" yWindow="1050" windowWidth="20550" windowHeight="18285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="585" yWindow="855" windowWidth="18405" windowHeight="18285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -97,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +108,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -148,12 +155,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -161,6 +192,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -2477,10 +2515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:X56"/>
+  <dimension ref="B2:X69"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11:P12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I65" sqref="E65:I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4626,6 +4664,120 @@
         <v>70673.975298032165</v>
       </c>
     </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="7">
+        <v>10000</v>
+      </c>
+      <c r="D64" s="7">
+        <v>10000</v>
+      </c>
+      <c r="E64" s="7">
+        <v>33</v>
+      </c>
+      <c r="F64" s="7">
+        <v>90</v>
+      </c>
+      <c r="G64" s="7">
+        <v>57.03</v>
+      </c>
+      <c r="H64" s="7">
+        <v>57</v>
+      </c>
+      <c r="I64" s="10">
+        <v>172.39599999999999</v>
+      </c>
+      <c r="J64" s="11">
+        <f t="shared" ref="J64:J65" si="12">(D64/I64)*1000</f>
+        <v>58005.986217777681</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="7">
+        <v>10000</v>
+      </c>
+      <c r="D65" s="7">
+        <v>10000</v>
+      </c>
+      <c r="E65" s="12">
+        <v>33</v>
+      </c>
+      <c r="F65" s="12">
+        <v>118</v>
+      </c>
+      <c r="G65" s="12">
+        <v>64.555700000000002</v>
+      </c>
+      <c r="H65" s="12">
+        <v>64</v>
+      </c>
+      <c r="I65" s="13">
+        <v>149.4589</v>
+      </c>
+      <c r="J65" s="11"/>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="7">
+        <v>10000</v>
+      </c>
+      <c r="D68" s="7">
+        <v>10000</v>
+      </c>
+      <c r="E68" s="7">
+        <v>47</v>
+      </c>
+      <c r="F68" s="7">
+        <v>99</v>
+      </c>
+      <c r="G68" s="7">
+        <v>70</v>
+      </c>
+      <c r="H68" s="7">
+        <v>70</v>
+      </c>
+      <c r="I68" s="10">
+        <v>140.70240000000001</v>
+      </c>
+      <c r="J68" s="11">
+        <f t="shared" ref="J68:J69" si="13">(D68/I68)*1000</f>
+        <v>71071.993086116505</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="7">
+        <v>10000</v>
+      </c>
+      <c r="D69" s="7">
+        <v>10000</v>
+      </c>
+      <c r="E69" s="12">
+        <v>36</v>
+      </c>
+      <c r="F69" s="12">
+        <v>410</v>
+      </c>
+      <c r="G69" s="12">
+        <v>55.37</v>
+      </c>
+      <c r="H69" s="12">
+        <v>54</v>
+      </c>
+      <c r="I69" s="13">
+        <v>172.5685</v>
+      </c>
+      <c r="J69" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4639,8 +4791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9051846-7276-40B2-9DDD-5F7652959633}">
   <dimension ref="B2:X65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4804,36 +4956,12 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="D6">
-        <v>1000</v>
-      </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>1000</v>
-      </c>
-      <c r="D7">
-        <v>1000</v>
-      </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J7" s="1"/>
       <c r="M7" s="2" t="s">
         <v>10</v>
       </c>
@@ -4842,20 +4970,22 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>1000</v>
-      </c>
-      <c r="D8">
-        <v>1000</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E8" s="8">
+        <v>488</v>
+      </c>
+      <c r="F8" s="8">
+        <v>590</v>
+      </c>
+      <c r="G8" s="8">
+        <v>500.52</v>
+      </c>
+      <c r="H8" s="8">
+        <v>498</v>
+      </c>
+      <c r="I8" s="9">
+        <v>19.945499999999999</v>
+      </c>
+      <c r="J8" s="1"/>
       <c r="M8" s="2" t="s">
         <v>11</v>
       </c>
@@ -5086,20 +5216,8 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15">
-        <v>1000</v>
-      </c>
-      <c r="D15">
-        <v>1000</v>
-      </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J15" s="1"/>
       <c r="M15" s="2" t="s">
         <v>9</v>
       </c>
@@ -5108,20 +5226,8 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16">
-        <v>1000</v>
-      </c>
-      <c r="D16">
-        <v>1000</v>
-      </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J16" s="1"/>
       <c r="M16" s="3" t="s">
         <v>12</v>
       </c>
@@ -5130,20 +5236,8 @@
       </c>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17">
-        <v>1000</v>
-      </c>
-      <c r="D17">
-        <v>1000</v>
-      </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J17" s="1"/>
       <c r="M17" t="s">
         <v>15</v>
       </c>
@@ -5383,20 +5477,8 @@
       </c>
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24">
-        <v>1000</v>
-      </c>
-      <c r="D24">
-        <v>1000</v>
-      </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J24" s="1"/>
       <c r="M24" s="2" t="s">
         <v>14</v>
       </c>
@@ -5411,20 +5493,8 @@
       </c>
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25">
-        <v>1000</v>
-      </c>
-      <c r="D25">
-        <v>1000</v>
-      </c>
       <c r="I25" s="1"/>
-      <c r="J25" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J25" s="1"/>
       <c r="M25" t="s">
         <v>15</v>
       </c>
@@ -5445,20 +5515,8 @@
       </c>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26">
-        <v>1000</v>
-      </c>
-      <c r="D26">
-        <v>1000</v>
-      </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J26" s="1"/>
       <c r="S26" s="3" t="s">
         <v>12</v>
       </c>
@@ -5704,20 +5762,8 @@
       <c r="X32" s="4"/>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33">
-        <v>1000</v>
-      </c>
-      <c r="D33">
-        <v>1000</v>
-      </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J33" s="1"/>
       <c r="M33" s="2" t="s">
         <v>10</v>
       </c>
@@ -5741,20 +5787,8 @@
       <c r="X33" s="4"/>
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34">
-        <v>1000</v>
-      </c>
-      <c r="D34">
-        <v>1000</v>
-      </c>
       <c r="I34" s="1"/>
-      <c r="J34" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J34" s="1"/>
       <c r="M34" s="2" t="s">
         <v>11</v>
       </c>
@@ -5772,20 +5806,22 @@
       </c>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35">
-        <v>1000</v>
-      </c>
-      <c r="D35">
-        <v>1000</v>
-      </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1" t="e">
-        <f t="shared" ref="J35:J56" si="9">(D35/I35)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E35" s="8">
+        <v>508</v>
+      </c>
+      <c r="F35" s="8">
+        <v>605</v>
+      </c>
+      <c r="G35" s="8">
+        <v>523.16510000000005</v>
+      </c>
+      <c r="H35" s="8">
+        <v>522</v>
+      </c>
+      <c r="I35" s="9">
+        <v>19.0687</v>
+      </c>
+      <c r="J35" s="1"/>
       <c r="M35" s="3" t="s">
         <v>12</v>
       </c>
@@ -5794,11 +5830,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O35" s="4" t="e">
-        <f t="shared" ref="O35:P35" si="10">(R35-R32)/R32</f>
+        <f t="shared" ref="O35:P35" si="9">(R35-R32)/R32</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P35" s="4" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5828,7 +5864,7 @@
         <v>19.286999999999999</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="J35:J56" si="10">(D36/I36)</f>
         <v>518.48395292165708</v>
       </c>
       <c r="M36" s="2" t="s">
@@ -5873,7 +5909,7 @@
         <v>19.266300000000001</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>519.04101981179565</v>
       </c>
       <c r="M37" s="2" t="s">
@@ -5918,7 +5954,7 @@
         <v>19.207799999999999</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>520.62183071460561</v>
       </c>
       <c r="M38" t="s">
@@ -5951,7 +5987,7 @@
         <v>15.951499999999999</v>
       </c>
       <c r="J39" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.2690029150863555</v>
       </c>
     </row>
@@ -5981,7 +6017,7 @@
         <v>16.04</v>
       </c>
       <c r="J40" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.2344139650872821</v>
       </c>
     </row>
@@ -6011,57 +6047,21 @@
         <v>15.9541</v>
       </c>
       <c r="J41" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.2679812712719611</v>
       </c>
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42">
-        <v>1000</v>
-      </c>
-      <c r="D42">
-        <v>1000</v>
-      </c>
       <c r="I42" s="1"/>
-      <c r="J42" s="1" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J42" s="1"/>
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43">
-        <v>1000</v>
-      </c>
-      <c r="D43">
-        <v>1000</v>
-      </c>
       <c r="I43" s="1"/>
-      <c r="J43" s="1" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J43" s="1"/>
     </row>
     <row r="44" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44">
-        <v>1000</v>
-      </c>
-      <c r="D44">
-        <v>1000</v>
-      </c>
       <c r="I44" s="1"/>
-      <c r="J44" s="1" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J44" s="1"/>
     </row>
     <row r="45" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -6089,7 +6089,7 @@
         <v>18.732299999999999</v>
       </c>
       <c r="J45" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>533.83727572161456</v>
       </c>
     </row>
@@ -6119,7 +6119,7 @@
         <v>18.7136</v>
       </c>
       <c r="J46" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>534.37072503419972</v>
       </c>
     </row>
@@ -6149,7 +6149,7 @@
         <v>18.798100000000002</v>
       </c>
       <c r="J47" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>531.96865640676447</v>
       </c>
       <c r="S47">
@@ -6185,7 +6185,7 @@
         <v>16.666499999999999</v>
       </c>
       <c r="J48" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.0000600006000067</v>
       </c>
     </row>
@@ -6215,7 +6215,7 @@
         <v>16.4528</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.0779928036565209</v>
       </c>
     </row>
@@ -6245,57 +6245,35 @@
         <v>16.498899999999999</v>
       </c>
       <c r="J50" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.0610101279479238</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51">
-        <v>1000</v>
-      </c>
-      <c r="D51">
-        <v>1000</v>
-      </c>
       <c r="I51" s="1"/>
-      <c r="J51" s="1" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J51" s="1"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52">
-        <v>1000</v>
-      </c>
-      <c r="D52">
-        <v>1000</v>
-      </c>
       <c r="I52" s="1"/>
-      <c r="J52" s="1" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J52" s="1"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53">
-        <v>1000</v>
-      </c>
-      <c r="D53">
-        <v>1000</v>
-      </c>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E53" s="8">
+        <v>506</v>
+      </c>
+      <c r="F53" s="8">
+        <v>642</v>
+      </c>
+      <c r="G53" s="8">
+        <v>521.75</v>
+      </c>
+      <c r="H53" s="8">
+        <v>521</v>
+      </c>
+      <c r="I53" s="9">
+        <v>19.130299999999998</v>
+      </c>
+      <c r="J53" s="1"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
@@ -6323,7 +6301,7 @@
         <v>19.2148</v>
       </c>
       <c r="J54" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>520.43216687136999</v>
       </c>
     </row>
@@ -6353,7 +6331,7 @@
         <v>19.340599999999998</v>
       </c>
       <c r="J55" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>517.04704093978478</v>
       </c>
     </row>
@@ -6383,7 +6361,7 @@
         <v>19.2729</v>
       </c>
       <c r="J56" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>518.863274338579</v>
       </c>
     </row>
@@ -6455,6 +6433,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>